<commit_message>
Clean and order combined data from Cuestionario CBDT and Sociodemográficos
</commit_message>
<xml_diff>
--- a/Data/Sociodemográficos.xlsx
+++ b/Data/Sociodemográficos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/935657b1b2443609/Research/Reports/ERC-CBDT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivan/Downloads/fwddatosestudionefrorein/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{E5A87A81-2FE0-AB43-926F-3389C757EE1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD2A39F7-738A-3242-AE5F-8FFA7D95BA86}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A87A81-2FE0-AB43-926F-3389C757EE1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="81">
   <si>
     <t>Num.</t>
   </si>
@@ -263,9 +263,6 @@
   </si>
   <si>
     <t>Q5</t>
-  </si>
-  <si>
-    <t>Escolaridad Papá</t>
   </si>
 </sst>
 </file>
@@ -642,7 +639,7 @@
   <dimension ref="A1:O100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -682,7 +679,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>81</v>
+        <v>6</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>7</v>

</xml_diff>